<commit_message>
Updated index and pastevents. Added WCFD material
</commit_message>
<xml_diff>
--- a/budget/budget2022.xlsx
+++ b/budget/budget2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rakul/Desktop/SWU/work/lillekat.github.io/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F18E3C-2701-EE4F-B7A7-4D984E8BF0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FEC5CC-5209-2746-AED3-EFDF79F18AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11060" yWindow="500" windowWidth="14540" windowHeight="14900" activeTab="1" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
   <si>
     <t>Lillekat 2022 budget</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>Balance</t>
+  </si>
+  <si>
+    <t>Støtte fra DDSA</t>
   </si>
 </sst>
 </file>
@@ -1528,10 +1531,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B219F9F2-A4CC-AD4F-A3F1-917E919B80E2}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="111" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1710,12 +1713,11 @@
       <c r="H6" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="L6" s="45">
-        <f>4000</f>
-        <v>4000</v>
+      <c r="K6" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="52">
+        <v>10000</v>
       </c>
       <c r="N6" s="51" t="s">
         <v>36</v>
@@ -1752,12 +1754,12 @@
         <f>E7*F7+G7</f>
         <v>5675</v>
       </c>
-      <c r="K7" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" s="50">
-        <f>SUM(L5+L6)</f>
-        <v>11873.75</v>
+      <c r="K7" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="45">
+        <f>4000</f>
+        <v>4000</v>
       </c>
       <c r="N7" s="44" t="s">
         <v>14</v>
@@ -1767,7 +1769,7 @@
         <v>14550</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
@@ -1793,8 +1795,15 @@
       <c r="H8" s="37" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K8" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="50">
+        <f>SUM(L5:L7)</f>
+        <v>21873.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
@@ -1822,10 +1831,6 @@
         <f>F9*E9+G9</f>
         <v>2171.4285714285716</v>
       </c>
-      <c r="K9" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" s="63"/>
       <c r="N9" s="62" t="s">
         <v>35</v>
       </c>
@@ -1848,12 +1853,10 @@
         <f>SUM(H4:H9)</f>
         <v>16317.857142857145</v>
       </c>
-      <c r="K10" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="L10" s="47">
-        <v>7908</v>
-      </c>
+      <c r="K10" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="63"/>
       <c r="N10" s="48" t="s">
         <v>34</v>
       </c>
@@ -1876,10 +1879,10 @@
         <v>16024.997142857144</v>
       </c>
       <c r="K11" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L11" s="47">
-        <v>0</v>
+        <v>7908</v>
       </c>
       <c r="N11" s="48" t="s">
         <v>33</v>
@@ -1890,10 +1893,10 @@
     </row>
     <row r="12" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="K12" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="L12" s="49" t="s">
-        <v>31</v>
+        <v>41</v>
+      </c>
+      <c r="L12" s="47">
+        <v>0</v>
       </c>
       <c r="N12" s="48" t="s">
         <v>32</v>
@@ -1904,9 +1907,11 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="K13" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="L13" s="49"/>
+        <v>42</v>
+      </c>
+      <c r="L13" s="49" t="s">
+        <v>31</v>
+      </c>
       <c r="N13" s="48"/>
       <c r="O13" s="49"/>
     </row>
@@ -1916,10 +1921,10 @@
       <c r="C14" s="40"/>
       <c r="D14" s="56"/>
       <c r="K14" s="48" t="s">
-        <v>44</v>
-      </c>
-      <c r="L14" s="47">
-        <v>0</v>
+        <v>43</v>
+      </c>
+      <c r="L14" s="49">
+        <v>7182</v>
       </c>
       <c r="N14" s="48" t="s">
         <v>30</v>
@@ -1930,10 +1935,10 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="57"/>
-      <c r="K15" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="L15" s="45">
+      <c r="K15" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="L15" s="47">
         <v>0</v>
       </c>
       <c r="N15" s="46" t="s">
@@ -1945,12 +1950,11 @@
     </row>
     <row r="16" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="57"/>
-      <c r="K16" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="L16" s="43">
-        <f>SUM(L10:L15)</f>
-        <v>7908</v>
+      <c r="K16" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="L16" s="45">
+        <v>0</v>
       </c>
       <c r="N16" s="44" t="s">
         <v>14</v>
@@ -1960,17 +1964,17 @@
         <v>6676.25</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="57"/>
-    </row>
-    <row r="18" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K18" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="L18" s="41">
-        <f>L7-L16</f>
-        <v>3965.75</v>
-      </c>
+      <c r="K17" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="43">
+        <f>SUM(L11:L16)</f>
+        <v>15090</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="N18" s="42" t="s">
         <v>28</v>
       </c>
@@ -1979,17 +1983,28 @@
         <v>7873.75</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="K19" s="54"/>
-      <c r="L19" s="55"/>
+    <row r="19" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="L19" s="41">
+        <f>L8-L17</f>
+        <v>6783.75</v>
+      </c>
       <c r="N19" s="54"/>
       <c r="O19" s="55"/>
     </row>
+    <row r="20" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="K20" s="54"/>
+      <c r="L20" s="55"/>
+    </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="K21" s="40" t="s">
+      <c r="N21" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="N21" s="40" t="s">
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K22" s="40" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2001,7 +2016,7 @@
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
LuciaKat added to photos. AoC material
</commit_message>
<xml_diff>
--- a/budget/budget2022.xlsx
+++ b/budget/budget2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rakul/Desktop/SWU/work/lillekat.github.io/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FEC5CC-5209-2746-AED3-EFDF79F18AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9BC61A-D597-4E4C-9978-1E710EFEAD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11060" yWindow="500" windowWidth="14540" windowHeight="14900" activeTab="1" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14900" activeTab="1" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
   </bookViews>
   <sheets>
     <sheet name="2022" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>Lillekat 2022 budget</t>
   </si>
@@ -104,12 +104,6 @@
   </si>
   <si>
     <t>Lillekat2022-09</t>
-  </si>
-  <si>
-    <t>Lillekat2022-10</t>
-  </si>
-  <si>
-    <t>Lillekat2022-11</t>
   </si>
   <si>
     <t>Lillekat 2023 budget</t>
@@ -600,7 +594,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -643,13 +637,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="5" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -669,8 +659,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1031,26 +1019,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="59"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="1:8" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -1235,10 +1223,10 @@
     </row>
     <row r="10" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="61"/>
+      <c r="C11" s="55"/>
       <c r="D11" s="22" t="s">
         <v>17</v>
       </c>
@@ -1379,10 +1367,10 @@
     </row>
     <row r="23" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="60" t="s">
+      <c r="B24" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="61"/>
+      <c r="C24" s="55"/>
       <c r="D24" s="22" t="s">
         <v>17</v>
       </c>
@@ -1531,10 +1519,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B219F9F2-A4CC-AD4F-A3F1-917E919B80E2}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="111" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="G2" zoomScale="135" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1553,26 +1541,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="58" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
+      <c r="A1" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="59"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1587,7 +1575,7 @@
       <c r="D3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="49" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="17" t="s">
@@ -1599,14 +1587,14 @@
       <c r="H3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" s="65"/>
-      <c r="N3" s="64" t="s">
-        <v>46</v>
-      </c>
-      <c r="O3" s="65"/>
+      <c r="K3" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="59"/>
+      <c r="N3" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" s="59"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1620,30 +1608,30 @@
         <v>96</v>
       </c>
       <c r="D4">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="E4" s="4">
         <f>C4/2.8</f>
         <v>34.285714285714285</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="32">
         <v>150</v>
       </c>
-      <c r="G4" s="35">
+      <c r="G4" s="33">
         <v>50</v>
       </c>
-      <c r="H4" s="37">
+      <c r="H4" s="34">
         <f>E4*F4</f>
         <v>5142.8571428571431</v>
       </c>
-      <c r="K4" s="62" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="63"/>
-      <c r="N4" s="62" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" s="63"/>
+      <c r="K4" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="57"/>
+      <c r="N4" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="57"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
@@ -1656,34 +1644,34 @@
         <f>51*1.2</f>
         <v>61.199999999999996</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
+      <c r="D5">
+        <v>73</v>
       </c>
       <c r="E5" s="4">
         <f>C5/2.8</f>
         <v>21.857142857142858</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="32">
         <v>150</v>
       </c>
-      <c r="G5" s="35">
+      <c r="G5" s="33">
         <v>50</v>
       </c>
-      <c r="H5" s="37">
+      <c r="H5" s="34">
         <f>E5*F5+G5</f>
         <v>3328.5714285714284</v>
       </c>
-      <c r="K5" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="52">
+      <c r="K5" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="48">
         <f>O18</f>
         <v>7873.75</v>
       </c>
-      <c r="N5" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="O5" s="52">
+      <c r="N5" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="48">
         <v>10000</v>
       </c>
     </row>
@@ -1698,31 +1686,31 @@
         <f>34*1.2</f>
         <v>40.799999999999997</v>
       </c>
-      <c r="D6" t="s">
-        <v>11</v>
+      <c r="D6">
+        <v>88</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="L6" s="52">
+      <c r="K6" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="48">
         <v>10000</v>
       </c>
-      <c r="N6" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="O6" s="45">
+      <c r="N6" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" s="41">
         <v>4550</v>
       </c>
     </row>
@@ -1737,286 +1725,229 @@
         <f>50*1.5</f>
         <v>75</v>
       </c>
-      <c r="D7" t="s">
-        <v>11</v>
+      <c r="D7">
+        <v>60</v>
       </c>
       <c r="E7" s="4">
         <f>C7/2</f>
         <v>37.5</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="32">
         <v>150</v>
       </c>
-      <c r="G7" s="35">
+      <c r="G7" s="33">
         <v>50</v>
       </c>
-      <c r="H7" s="37">
+      <c r="H7" s="34">
         <f>E7*F7+G7</f>
         <v>5675</v>
       </c>
-      <c r="K7" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="L7" s="45">
+      <c r="K7" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="41">
         <f>4000</f>
         <v>4000</v>
       </c>
-      <c r="N7" s="44" t="s">
+      <c r="N7" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="50">
+      <c r="O7" s="46">
         <f>SUM(O5+O6)</f>
         <v>14550</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="7">
-        <v>44876</v>
-      </c>
-      <c r="C8" s="4">
-        <f>30*1.2</f>
-        <v>36</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="44" t="s">
+      <c r="A8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="50">
+      <c r="B8" s="20"/>
+      <c r="C8" s="35">
+        <f>SUM(C4:C7)</f>
+        <v>273</v>
+      </c>
+      <c r="D8" s="20">
+        <f>SUM(D4:D7)</f>
+        <v>336</v>
+      </c>
+      <c r="E8" s="20"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21">
+        <f>SUM(H4:H7)</f>
+        <v>14146.428571428572</v>
+      </c>
+      <c r="K8" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="46">
         <f>SUM(L5:L7)</f>
         <v>21873.75</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="11">
-        <v>44890</v>
-      </c>
-      <c r="C9" s="13">
-        <f>33*1.2</f>
-        <v>39.6</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="4">
-        <f>C9/2.8</f>
-        <v>14.142857142857144</v>
-      </c>
-      <c r="F9" s="34">
-        <v>150</v>
-      </c>
-      <c r="G9" s="36">
-        <v>50</v>
-      </c>
-      <c r="H9" s="38">
-        <f>F9*E9+G9</f>
-        <v>2171.4285714285716</v>
-      </c>
-      <c r="N9" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="O9" s="63"/>
-    </row>
-    <row r="10" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21">
+        <f>H8-292.86</f>
+        <v>13853.568571428572</v>
+      </c>
+      <c r="N9" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="57"/>
+    </row>
+    <row r="10" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="K10" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="L10" s="57"/>
+      <c r="N10" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" s="43">
+        <v>501.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K11" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="43">
+        <v>7908</v>
+      </c>
+      <c r="N11" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="O11" s="43">
+        <v>2611.1999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="36"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="50"/>
+      <c r="K12" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="43">
+        <v>0</v>
+      </c>
+      <c r="N12" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="O12" s="45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="51"/>
+      <c r="K13" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13" s="44"/>
+      <c r="O13" s="45"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="51"/>
+      <c r="K14" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="L14" s="45">
+        <v>7182</v>
+      </c>
+      <c r="N14" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" s="43">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="51"/>
+      <c r="K15" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="L15" s="43">
+        <v>0</v>
+      </c>
+      <c r="N15" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="O15" s="41">
+        <v>584.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="L16" s="41">
+        <v>0</v>
+      </c>
+      <c r="N16" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="39">
-        <f>SUM(C4:C9)</f>
-        <v>348.6</v>
-      </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21">
-        <f>SUM(H4:H9)</f>
-        <v>16317.857142857145</v>
-      </c>
-      <c r="K10" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="63"/>
-      <c r="N10" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="O10" s="47">
-        <v>501.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21">
-        <f>H10-292.86</f>
-        <v>16024.997142857144</v>
-      </c>
-      <c r="K11" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="L11" s="47">
-        <v>7908</v>
-      </c>
-      <c r="N11" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="O11" s="47">
-        <v>2611.1999999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="K12" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="L12" s="47">
-        <v>0</v>
-      </c>
-      <c r="N12" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="O12" s="49" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="K13" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="L13" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="N13" s="48"/>
-      <c r="O13" s="49"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="40"/>
-      <c r="B14" s="56"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="56"/>
-      <c r="K14" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="L14" s="49">
-        <v>7182</v>
-      </c>
-      <c r="N14" s="48" t="s">
-        <v>30</v>
-      </c>
-      <c r="O14" s="47">
-        <v>2979</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="57"/>
-      <c r="K15" s="48" t="s">
-        <v>44</v>
-      </c>
-      <c r="L15" s="47">
-        <v>0</v>
-      </c>
-      <c r="N15" s="46" t="s">
-        <v>29</v>
-      </c>
-      <c r="O15" s="45">
-        <v>584.75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="57"/>
-      <c r="K16" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="L16" s="45">
-        <v>0</v>
-      </c>
-      <c r="N16" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="O16" s="43">
+      <c r="O16" s="39">
         <f>SUM(O10:O15)</f>
         <v>6676.25</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="57"/>
-      <c r="K17" s="44" t="s">
+    <row r="17" spans="11:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="L17" s="43">
+      <c r="L17" s="39">
         <f>SUM(L11:L16)</f>
         <v>15090</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="N18" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="O18" s="41">
+    <row r="18" spans="11:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N18" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="O18" s="37">
         <f>O7-O16</f>
         <v>7873.75</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K19" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="L19" s="41">
+    <row r="19" spans="11:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="L19" s="37">
         <f>L8-L17</f>
         <v>6783.75</v>
       </c>
-      <c r="N19" s="54"/>
-      <c r="O19" s="55"/>
-    </row>
-    <row r="20" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="K20" s="54"/>
-      <c r="L20" s="55"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="N21" s="40" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="K22" s="40" t="s">
-        <v>27</v>
+      <c r="N19" s="36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="11:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="K20" s="36" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="N9:O9"/>
     <mergeCell ref="A1:H2"/>
     <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N9:O9"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K10:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>